<commit_message>
fixes for datasets, new vis examples
</commit_message>
<xml_diff>
--- a/data/data-planning.xlsx
+++ b/data/data-planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/az49/Dropbox/personal-temp/vis4dsr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C67FA33-7C67-3E43-993C-8221DDAEEC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4404D9A-C039-8A43-B4FB-9372FB2DDEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{311AB05F-48C8-AD42-AFF2-4C2014B933C5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>how to read visualizations</t>
   </si>
@@ -187,9 +187,6 @@
     <t>coral_resilience (experiment)</t>
   </si>
   <si>
-    <t>IASGE survey</t>
-  </si>
-  <si>
     <t>dozens, including binary, ordered/unordered factor, and free text</t>
   </si>
   <si>
@@ -215,6 +212,21 @@
   </si>
   <si>
     <t>could group and count</t>
+  </si>
+  <si>
+    <t>affinity spending</t>
+  </si>
+  <si>
+    <t>1, but could pivot wider to compare across spending categories?</t>
+  </si>
+  <si>
+    <t>spending category and income quartile, but spending category might includes some categories that could be grouped?</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>git_experience</t>
   </si>
 </sst>
 </file>
@@ -612,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B63744F-B459-2A4A-90E5-0A721DEC1E71}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -847,10 +859,10 @@
   <dimension ref="A1:XFC18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" activeCellId="1" sqref="F6 F10"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,7 +873,8 @@
     <col min="4" max="4" width="54.1640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="44.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="15" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="15" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16383" x14ac:dyDescent="0.2">
@@ -872,13 +885,16 @@
         <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:16383" x14ac:dyDescent="0.2">
@@ -892,13 +908,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:16383" x14ac:dyDescent="0.2">
@@ -912,13 +931,16 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="5">
         <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:16383" x14ac:dyDescent="0.2">
@@ -932,10 +954,13 @@
         <v>48</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="5">
         <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:16383" x14ac:dyDescent="0.2">
@@ -946,7 +971,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="5">
         <v>1</v>
@@ -976,6 +1001,9 @@
       <c r="F11" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="G11" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:16383" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -985,6 +1013,9 @@
         <v>44</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -999,6 +1030,9 @@
         <v>44</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1016,6 +1050,9 @@
         <v>44</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>